<commit_message>
1103 - new table
</commit_message>
<xml_diff>
--- a/others/Web-Page-Design-i18n.xlsx
+++ b/others/Web-Page-Design-i18n.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="237">
   <si>
     <t>index</t>
   </si>
@@ -43,10 +43,13 @@
     <t>dataForm</t>
   </si>
   <si>
+    <t>A02</t>
+  </si>
+  <si>
     <t>primaryKey</t>
   </si>
   <si>
-    <t>A02</t>
+    <t>A03</t>
   </si>
   <si>
     <t>dateOfApplication</t>
@@ -58,7 +61,7 @@
     <t>申請日期</t>
   </si>
   <si>
-    <t>B00</t>
+    <t>B01</t>
   </si>
   <si>
     <t>applyFor</t>
@@ -73,7 +76,7 @@
     <t>申請項目</t>
   </si>
   <si>
-    <t>C00</t>
+    <t>C01</t>
   </si>
   <si>
     <t>applicant</t>
@@ -88,7 +91,7 @@
     <t>申請人</t>
   </si>
   <si>
-    <t>C01</t>
+    <t>C02</t>
   </si>
   <si>
     <t>identityCardNumber</t>
@@ -97,7 +100,7 @@
     <t>身分證字號</t>
   </si>
   <si>
-    <t>C02</t>
+    <t>C03</t>
   </si>
   <si>
     <t>contactNumber</t>
@@ -106,7 +109,7 @@
     <t>連絡電話</t>
   </si>
   <si>
-    <t>C03</t>
+    <t>C04</t>
   </si>
   <si>
     <t>phoneNumber</t>
@@ -115,7 +118,7 @@
     <t>手機號碼</t>
   </si>
   <si>
-    <t>C04</t>
+    <t>C05</t>
   </si>
   <si>
     <t>residence</t>
@@ -124,7 +127,7 @@
     <t>居住縣市</t>
   </si>
   <si>
-    <t>C05</t>
+    <t>C06</t>
   </si>
   <si>
     <t>address</t>
@@ -133,12 +136,66 @@
     <t>通訊地址</t>
   </si>
   <si>
+    <t>N00</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>P00</t>
+  </si>
+  <si>
+    <t>P01</t>
+  </si>
+  <si>
+    <t>dataMember</t>
+  </si>
+  <si>
+    <t>P02</t>
+  </si>
+  <si>
+    <t>P03</t>
+  </si>
+  <si>
+    <t>accountCreationDate</t>
+  </si>
+  <si>
+    <t>帳號創建日期</t>
+  </si>
+  <si>
+    <t>Q01</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>member</t>
+  </si>
+  <si>
+    <t>使用者名稱</t>
+  </si>
+  <si>
+    <t>Q02</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>密碼</t>
+  </si>
+  <si>
+    <t>Q03</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>電子郵件</t>
+  </si>
+  <si>
     <t>Z00</t>
   </si>
   <si>
-    <t>END</t>
-  </si>
-  <si>
     <t>Chinese</t>
   </si>
   <si>
@@ -392,6 +449,24 @@
   </si>
   <si>
     <t>Address</t>
+  </si>
+  <si>
+    <t>dataMemberUsernameMemberText</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>dataMemberPasswordMemberText</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>dataMemberEmailMemberText</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
   <si>
     <t>firstTime</t>
@@ -695,7 +770,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -718,6 +793,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -947,10 +1025,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="28.88"/>
-    <col customWidth="1" min="3" max="3" width="7.88"/>
-    <col customWidth="1" min="4" max="4" width="15.25"/>
-    <col customWidth="1" min="5" max="5" width="6.25"/>
+    <col customWidth="1" min="1" max="1" width="30.0"/>
+    <col customWidth="1" min="3" max="3" width="10.38"/>
+    <col customWidth="1" min="4" max="4" width="16.63"/>
+    <col customWidth="1" min="5" max="5" width="7.13"/>
     <col customWidth="1" min="6" max="6" width="7.75"/>
   </cols>
   <sheetData>
@@ -969,7 +1047,10 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="str">
+        <f t="shared" ref="A3:A25" si="1"> if(C3 &lt;&gt; "", C3 &amp; replace(D3,1,1, UPPER(LEFT(D3,1))) &amp; replace(E3,1,1, UPPER(LEFT(E3,1))) &amp; replace(F3,1,1, UPPER(LEFT(F3,1))), C3)</f>
+        <v/>
+      </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -988,7 +1069,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="str">
-        <f t="shared" ref="A4:A19" si="1"> if(C4 = "dataForm", C4 &amp; replace(D4,1,1, UPPER(LEFT(D4,1))) &amp; replace(E4,1,1, UPPER(LEFT(E4,1))) &amp; replace(F4,1,1, UPPER(LEFT(F4,1))), C4)</f>
+        <f t="shared" si="1"/>
         <v>START</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1002,7 +1083,7 @@
     <row r="5">
       <c r="A5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>dataFormPrimaryKey</v>
+        <v>dataForm</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
@@ -1010,270 +1091,425 @@
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>dataFormDateOfApplicationDate</v>
+        <v>dataFormPrimaryKey</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>dataFormApplyForPurposeChoice</v>
+        <v>dataFormDateOfApplicationDate</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>dataFormApplicantFormText</v>
+        <v>dataFormApplyForPurposeChoice</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>20</v>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>dataFormIdentityCardNumberFormText</v>
+        <v>dataFormApplicantFormText</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>dataFormContactNumberFormText</v>
+        <v>dataFormIdentityCardNumberFormText</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>dataFormPhoneNumberFormText</v>
+        <v>dataFormContactNumberFormText</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>dataFormResidenceFormChoice</v>
+        <v>dataFormPhoneNumberFormText</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>dataFormAddressFormText</v>
+        <v>dataFormResidenceFormChoice</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>END</v>
+        <v>dataFormAddressFormText</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
+        <v>END</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
+        <v>START</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
+        <v>dataMember</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="str">
         <f t="shared" si="1"/>
+        <v>dataMemberPrimaryKey</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>dataMemberAccountCreationDateDate</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>dataMemberUsernameMemberText</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>dataMemberPasswordMemberText</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>dataMemberEmailMemberText</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>END</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="1"/>
-    </row>
     <row r="26">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1" t="str">
+        <f t="shared" ref="A26:A29" si="2"> if(C26 = "dataForm", C26 &amp; replace(D26,1,1, UPPER(LEFT(D26,1))) &amp; replace(E26,1,1, UPPER(LEFT(E26,1))) &amp; replace(F26,1,1, UPPER(LEFT(F26,1))), C26)</f>
+        <v/>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1"/>
@@ -1796,6 +2032,36 @@
     </row>
     <row r="203">
       <c r="A203" s="1"/>
+    </row>
+    <row r="204">
+      <c r="A204" s="1"/>
+    </row>
+    <row r="205">
+      <c r="A205" s="1"/>
+    </row>
+    <row r="206">
+      <c r="A206" s="1"/>
+    </row>
+    <row r="207">
+      <c r="A207" s="1"/>
+    </row>
+    <row r="208">
+      <c r="A208" s="1"/>
+    </row>
+    <row r="209">
+      <c r="A209" s="1"/>
+    </row>
+    <row r="210">
+      <c r="A210" s="1"/>
+    </row>
+    <row r="211">
+      <c r="A211" s="1"/>
+    </row>
+    <row r="212">
+      <c r="A212" s="1"/>
+    </row>
+    <row r="213">
+      <c r="A213" s="1"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1812,7 +2078,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="109.75"/>
+    <col customWidth="1" min="1" max="1" width="68.0"/>
     <col customWidth="1" min="2" max="2" width="28.88"/>
   </cols>
   <sheetData>
@@ -1824,15 +2090,14 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
-        <f t="shared" ref="A3:A15" si="1"> if(C3 = "index", "&lt;?php $tableQuery = &lt;&lt;&lt;EOD", 
-  if(C3 = "A00", ""&amp;REPT(char(32), 4)&amp;"CREATE TABLE IF NOT EXISTS `dataform` (",
-  if(C3 = "Z00", ""&amp;REPT(char(32), 4)&amp;") ENGINE=InnoDB DEFAULT CHARSET=utf8 COLLATE=utf8_general_ci;",
+        <f t="shared" ref="A3:A26" si="1"> if(C3 = "index", "&lt;?php $tableQuery = &lt;&lt;&lt;EOD", 
+  if(or(C3 = "A01", C3 = "P01"), ""&amp;REPT(char(32), 4)&amp;"CREATE TABLE IF NOT EXISTS `"&amp;LOWER($B3)&amp;"` (",
+  if(or(C3 = "N00", C3 = "Z00"), ""&amp;REPT(char(32), 4)&amp;") ENGINE=InnoDB DEFAULT CHARSET=utf8 COLLATE=utf8_general_ci;",
   if(E3 = "primaryKey", ""&amp;REPT(char(32), 8)&amp;"`"&amp;B3&amp;"` int(64) NOT NULL,",
-  if(E3 = "dateOfApplication",  ""&amp;REPT(char(32), 8)&amp;"`"&amp;B3&amp;"` timestamp NOT NULL DEFAULT current_timestamp() ON UPDATE current_timestamp() COMMENT '"&amp;H3&amp;"',",
-  if(E3 = "applyFor", ""&amp;REPT(char(32), 8)&amp;"`"&amp;B3&amp;"` tinytext NOT NULL COMMENT '"&amp;H3&amp;"',",
-  if(and(F3 = "form", C4 = "Z00"), ""&amp;REPT(char(32), 8)&amp;"`"&amp;B3&amp;"` tinytext NOT NULL COMMENT '"&amp;H3&amp;"'",
-  if(F3 = "form", ""&amp;REPT(char(32), 8)&amp;"`"&amp;B3&amp;"` tinytext NOT NULL COMMENT '"&amp;H3&amp;"',",
-  if(C2 = "Z00", "EOD ?&gt;", "")))))))))</f>
+  if(or(E3 = "dateOfApplication", E3 = "accountCreationDate"),  ""&amp;REPT(char(32), 8)&amp;"`"&amp;B3&amp;"` timestamp NOT NULL DEFAULT current_timestamp() ON UPDATE current_timestamp() COMMENT '"&amp;H3&amp;"',",
+  if(and(or(G3 = "choice", G3 = "text"), or(C4 = "N00", C4 = "Z00")), ""&amp;REPT(char(32), 8)&amp;"`"&amp;B3&amp;"` tinytext NOT NULL COMMENT '"&amp;H3&amp;"'",
+  if(or(G3 = "choice", G3 = "text"), ""&amp;REPT(char(32), 8)&amp;"`"&amp;B3&amp;"` tinytext NOT NULL COMMENT '"&amp;H3&amp;"',",
+  if(and(or(C2 = "N00", C2 = "Z00"), C4 = ""), "EOD ?&gt;", ""))))))))</f>
         <v>&lt;?php $tableQuery = &lt;&lt;&lt;EOD</v>
       </c>
       <c r="B3" s="4" t="str">
@@ -1867,7 +2132,7 @@
     <row r="4">
       <c r="A4" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>    CREATE TABLE IF NOT EXISTS `dataform` (</v>
+        <v/>
       </c>
       <c r="B4" s="4" t="str">
         <f>columns!A4</f>
@@ -1901,11 +2166,11 @@
     <row r="5">
       <c r="A5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>        `dataFormPrimaryKey` int(64) NOT NULL,</v>
+        <v>    CREATE TABLE IF NOT EXISTS `dataform` (</v>
       </c>
       <c r="B5" s="4" t="str">
         <f>columns!A5</f>
-        <v>dataFormPrimaryKey</v>
+        <v>dataForm</v>
       </c>
       <c r="C5" s="4" t="str">
         <f>columns!B5</f>
@@ -1917,7 +2182,7 @@
       </c>
       <c r="E5" s="4" t="str">
         <f>columns!D5</f>
-        <v>primaryKey</v>
+        <v/>
       </c>
       <c r="F5" s="4" t="str">
         <f>columns!E5</f>
@@ -1935,11 +2200,11 @@
     <row r="6">
       <c r="A6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>        `dataFormDateOfApplicationDate` timestamp NOT NULL DEFAULT current_timestamp() ON UPDATE current_timestamp() COMMENT '申請日期',</v>
+        <v>        `dataFormPrimaryKey` int(64) NOT NULL,</v>
       </c>
       <c r="B6" s="4" t="str">
         <f>columns!A6</f>
-        <v>dataFormDateOfApplicationDate</v>
+        <v>dataFormPrimaryKey</v>
       </c>
       <c r="C6" s="4" t="str">
         <f>columns!B6</f>
@@ -1951,7 +2216,7 @@
       </c>
       <c r="E6" s="4" t="str">
         <f>columns!D6</f>
-        <v>dateOfApplication</v>
+        <v>primaryKey</v>
       </c>
       <c r="F6" s="4" t="str">
         <f>columns!E6</f>
@@ -1959,25 +2224,25 @@
       </c>
       <c r="G6" s="4" t="str">
         <f>columns!F6</f>
-        <v>date</v>
+        <v/>
       </c>
       <c r="H6" s="4" t="str">
         <f>columns!G6</f>
-        <v>申請日期</v>
+        <v/>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>        `dataFormApplyForPurposeChoice` tinytext NOT NULL COMMENT '申請項目',</v>
+        <v>        `dataFormDateOfApplicationDate` timestamp NOT NULL DEFAULT current_timestamp() ON UPDATE current_timestamp() COMMENT '申請日期',</v>
       </c>
       <c r="B7" s="4" t="str">
         <f>columns!A7</f>
-        <v>dataFormApplyForPurposeChoice</v>
+        <v>dataFormDateOfApplicationDate</v>
       </c>
       <c r="C7" s="4" t="str">
         <f>columns!B7</f>
-        <v>B00</v>
+        <v>A03</v>
       </c>
       <c r="D7" s="4" t="str">
         <f>columns!C7</f>
@@ -1985,33 +2250,33 @@
       </c>
       <c r="E7" s="4" t="str">
         <f>columns!D7</f>
-        <v>applyFor</v>
+        <v>dateOfApplication</v>
       </c>
       <c r="F7" s="4" t="str">
         <f>columns!E7</f>
-        <v>purpose</v>
+        <v/>
       </c>
       <c r="G7" s="4" t="str">
         <f>columns!F7</f>
-        <v>choice</v>
+        <v>date</v>
       </c>
       <c r="H7" s="4" t="str">
         <f>columns!G7</f>
-        <v>申請項目</v>
+        <v>申請日期</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>        `dataFormApplicantFormText` tinytext NOT NULL COMMENT '申請人',</v>
+        <v>        `dataFormApplyForPurposeChoice` tinytext NOT NULL COMMENT '申請項目',</v>
       </c>
       <c r="B8" s="4" t="str">
         <f>columns!A8</f>
-        <v>dataFormApplicantFormText</v>
+        <v>dataFormApplyForPurposeChoice</v>
       </c>
       <c r="C8" s="4" t="str">
         <f>columns!B8</f>
-        <v>C00</v>
+        <v>B01</v>
       </c>
       <c r="D8" s="4" t="str">
         <f>columns!C8</f>
@@ -2019,29 +2284,29 @@
       </c>
       <c r="E8" s="4" t="str">
         <f>columns!D8</f>
-        <v>applicant</v>
+        <v>applyFor</v>
       </c>
       <c r="F8" s="4" t="str">
         <f>columns!E8</f>
-        <v>form</v>
+        <v>purpose</v>
       </c>
       <c r="G8" s="4" t="str">
         <f>columns!F8</f>
-        <v>text</v>
+        <v>choice</v>
       </c>
       <c r="H8" s="4" t="str">
         <f>columns!G8</f>
-        <v>申請人</v>
+        <v>申請項目</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>        `dataFormIdentityCardNumberFormText` tinytext NOT NULL COMMENT '身分證字號',</v>
+        <v>        `dataFormApplicantFormText` tinytext NOT NULL COMMENT '申請人',</v>
       </c>
       <c r="B9" s="4" t="str">
         <f>columns!A9</f>
-        <v>dataFormIdentityCardNumberFormText</v>
+        <v>dataFormApplicantFormText</v>
       </c>
       <c r="C9" s="4" t="str">
         <f>columns!B9</f>
@@ -2053,7 +2318,7 @@
       </c>
       <c r="E9" s="4" t="str">
         <f>columns!D9</f>
-        <v>identityCardNumber</v>
+        <v>applicant</v>
       </c>
       <c r="F9" s="4" t="str">
         <f>columns!E9</f>
@@ -2065,17 +2330,17 @@
       </c>
       <c r="H9" s="4" t="str">
         <f>columns!G9</f>
-        <v>身分證字號</v>
+        <v>申請人</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>        `dataFormContactNumberFormText` tinytext NOT NULL COMMENT '連絡電話',</v>
+        <v>        `dataFormIdentityCardNumberFormText` tinytext NOT NULL COMMENT '身分證字號',</v>
       </c>
       <c r="B10" s="4" t="str">
         <f>columns!A10</f>
-        <v>dataFormContactNumberFormText</v>
+        <v>dataFormIdentityCardNumberFormText</v>
       </c>
       <c r="C10" s="4" t="str">
         <f>columns!B10</f>
@@ -2087,7 +2352,7 @@
       </c>
       <c r="E10" s="4" t="str">
         <f>columns!D10</f>
-        <v>contactNumber</v>
+        <v>identityCardNumber</v>
       </c>
       <c r="F10" s="4" t="str">
         <f>columns!E10</f>
@@ -2099,17 +2364,17 @@
       </c>
       <c r="H10" s="4" t="str">
         <f>columns!G10</f>
-        <v>連絡電話</v>
+        <v>身分證字號</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>        `dataFormPhoneNumberFormText` tinytext NOT NULL COMMENT '手機號碼',</v>
+        <v>        `dataFormContactNumberFormText` tinytext NOT NULL COMMENT '連絡電話',</v>
       </c>
       <c r="B11" s="4" t="str">
         <f>columns!A11</f>
-        <v>dataFormPhoneNumberFormText</v>
+        <v>dataFormContactNumberFormText</v>
       </c>
       <c r="C11" s="4" t="str">
         <f>columns!B11</f>
@@ -2121,7 +2386,7 @@
       </c>
       <c r="E11" s="4" t="str">
         <f>columns!D11</f>
-        <v>phoneNumber</v>
+        <v>contactNumber</v>
       </c>
       <c r="F11" s="4" t="str">
         <f>columns!E11</f>
@@ -2133,17 +2398,17 @@
       </c>
       <c r="H11" s="4" t="str">
         <f>columns!G11</f>
-        <v>手機號碼</v>
+        <v>連絡電話</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>        `dataFormResidenceFormChoice` tinytext NOT NULL COMMENT '居住縣市',</v>
+        <v>        `dataFormPhoneNumberFormText` tinytext NOT NULL COMMENT '手機號碼',</v>
       </c>
       <c r="B12" s="4" t="str">
         <f>columns!A12</f>
-        <v>dataFormResidenceFormChoice</v>
+        <v>dataFormPhoneNumberFormText</v>
       </c>
       <c r="C12" s="4" t="str">
         <f>columns!B12</f>
@@ -2155,7 +2420,7 @@
       </c>
       <c r="E12" s="4" t="str">
         <f>columns!D12</f>
-        <v>residence</v>
+        <v>phoneNumber</v>
       </c>
       <c r="F12" s="4" t="str">
         <f>columns!E12</f>
@@ -2163,21 +2428,21 @@
       </c>
       <c r="G12" s="4" t="str">
         <f>columns!F12</f>
-        <v>choice</v>
+        <v>text</v>
       </c>
       <c r="H12" s="4" t="str">
         <f>columns!G12</f>
-        <v>居住縣市</v>
+        <v>手機號碼</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>        `dataFormAddressFormText` tinytext NOT NULL COMMENT '通訊地址'</v>
+        <v>        `dataFormResidenceFormChoice` tinytext NOT NULL COMMENT '居住縣市',</v>
       </c>
       <c r="B13" s="4" t="str">
         <f>columns!A13</f>
-        <v>dataFormAddressFormText</v>
+        <v>dataFormResidenceFormChoice</v>
       </c>
       <c r="C13" s="4" t="str">
         <f>columns!B13</f>
@@ -2189,7 +2454,7 @@
       </c>
       <c r="E13" s="4" t="str">
         <f>columns!D13</f>
-        <v>address</v>
+        <v>residence</v>
       </c>
       <c r="F13" s="4" t="str">
         <f>columns!E13</f>
@@ -2197,81 +2462,454 @@
       </c>
       <c r="G13" s="4" t="str">
         <f>columns!F13</f>
-        <v>text</v>
+        <v>choice</v>
       </c>
       <c r="H13" s="4" t="str">
         <f>columns!G13</f>
-        <v>通訊地址</v>
+        <v>居住縣市</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>    ) ENGINE=InnoDB DEFAULT CHARSET=utf8 COLLATE=utf8_general_ci;</v>
+        <v>        `dataFormAddressFormText` tinytext NOT NULL COMMENT '通訊地址'</v>
       </c>
       <c r="B14" s="4" t="str">
         <f>columns!A14</f>
-        <v>END</v>
+        <v>dataFormAddressFormText</v>
       </c>
       <c r="C14" s="4" t="str">
         <f>columns!B14</f>
-        <v>Z00</v>
+        <v>C06</v>
       </c>
       <c r="D14" s="4" t="str">
         <f>columns!C14</f>
-        <v>END</v>
+        <v>dataForm</v>
       </c>
       <c r="E14" s="4" t="str">
         <f>columns!D14</f>
-        <v/>
+        <v>address</v>
       </c>
       <c r="F14" s="4" t="str">
         <f>columns!E14</f>
-        <v/>
+        <v>form</v>
       </c>
       <c r="G14" s="4" t="str">
         <f>columns!F14</f>
-        <v/>
+        <v>text</v>
+      </c>
+      <c r="H14" s="4" t="str">
+        <f>columns!G14</f>
+        <v>通訊地址</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="str">
         <f t="shared" si="1"/>
+        <v>    ) ENGINE=InnoDB DEFAULT CHARSET=utf8 COLLATE=utf8_general_ci;</v>
+      </c>
+      <c r="B15" s="4" t="str">
+        <f>columns!A15</f>
+        <v>END</v>
+      </c>
+      <c r="C15" s="4" t="str">
+        <f>columns!B15</f>
+        <v>N00</v>
+      </c>
+      <c r="D15" s="4" t="str">
+        <f>columns!C15</f>
+        <v>END</v>
+      </c>
+      <c r="E15" s="4" t="str">
+        <f>columns!D15</f>
+        <v/>
+      </c>
+      <c r="F15" s="4" t="str">
+        <f>columns!E15</f>
+        <v/>
+      </c>
+      <c r="G15" s="4" t="str">
+        <f>columns!F15</f>
+        <v/>
+      </c>
+      <c r="H15" s="4" t="str">
+        <f>columns!G15</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B16" s="4" t="str">
+        <f>columns!A16</f>
+        <v/>
+      </c>
+      <c r="C16" s="4" t="str">
+        <f>columns!B16</f>
+        <v/>
+      </c>
+      <c r="D16" s="4" t="str">
+        <f>columns!C16</f>
+        <v/>
+      </c>
+      <c r="E16" s="4" t="str">
+        <f>columns!D16</f>
+        <v/>
+      </c>
+      <c r="F16" s="4" t="str">
+        <f>columns!E16</f>
+        <v/>
+      </c>
+      <c r="G16" s="4" t="str">
+        <f>columns!F16</f>
+        <v/>
+      </c>
+      <c r="H16" s="4" t="str">
+        <f>columns!G16</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B17" s="4" t="str">
+        <f>columns!A17</f>
+        <v>START</v>
+      </c>
+      <c r="C17" s="4" t="str">
+        <f>columns!B17</f>
+        <v>P00</v>
+      </c>
+      <c r="D17" s="4" t="str">
+        <f>columns!C17</f>
+        <v>START</v>
+      </c>
+      <c r="E17" s="4" t="str">
+        <f>columns!D17</f>
+        <v/>
+      </c>
+      <c r="F17" s="4" t="str">
+        <f>columns!E17</f>
+        <v/>
+      </c>
+      <c r="G17" s="4" t="str">
+        <f>columns!F17</f>
+        <v/>
+      </c>
+      <c r="H17" s="4" t="str">
+        <f>columns!G17</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>    CREATE TABLE IF NOT EXISTS `datamember` (</v>
+      </c>
+      <c r="B18" s="4" t="str">
+        <f>columns!A18</f>
+        <v>dataMember</v>
+      </c>
+      <c r="C18" s="4" t="str">
+        <f>columns!B18</f>
+        <v>P01</v>
+      </c>
+      <c r="D18" s="4" t="str">
+        <f>columns!C18</f>
+        <v>dataMember</v>
+      </c>
+      <c r="E18" s="4" t="str">
+        <f>columns!D18</f>
+        <v/>
+      </c>
+      <c r="F18" s="4" t="str">
+        <f>columns!E18</f>
+        <v/>
+      </c>
+      <c r="G18" s="4" t="str">
+        <f>columns!F18</f>
+        <v/>
+      </c>
+      <c r="H18" s="4" t="str">
+        <f>columns!G18</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>        `dataMemberPrimaryKey` int(64) NOT NULL,</v>
+      </c>
+      <c r="B19" s="4" t="str">
+        <f>columns!A19</f>
+        <v>dataMemberPrimaryKey</v>
+      </c>
+      <c r="C19" s="4" t="str">
+        <f>columns!B19</f>
+        <v>P02</v>
+      </c>
+      <c r="D19" s="4" t="str">
+        <f>columns!C19</f>
+        <v>dataMember</v>
+      </c>
+      <c r="E19" s="4" t="str">
+        <f>columns!D19</f>
+        <v>primaryKey</v>
+      </c>
+      <c r="F19" s="4" t="str">
+        <f>columns!E19</f>
+        <v/>
+      </c>
+      <c r="G19" s="4" t="str">
+        <f>columns!F19</f>
+        <v/>
+      </c>
+      <c r="H19" s="4" t="str">
+        <f>columns!G19</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>        `dataMemberAccountCreationDateDate` timestamp NOT NULL DEFAULT current_timestamp() ON UPDATE current_timestamp() COMMENT '帳號創建日期',</v>
+      </c>
+      <c r="B20" s="4" t="str">
+        <f>columns!A20</f>
+        <v>dataMemberAccountCreationDateDate</v>
+      </c>
+      <c r="C20" s="4" t="str">
+        <f>columns!B20</f>
+        <v>P03</v>
+      </c>
+      <c r="D20" s="4" t="str">
+        <f>columns!C20</f>
+        <v>dataMember</v>
+      </c>
+      <c r="E20" s="4" t="str">
+        <f>columns!D20</f>
+        <v>accountCreationDate</v>
+      </c>
+      <c r="F20" s="4" t="str">
+        <f>columns!E20</f>
+        <v/>
+      </c>
+      <c r="G20" s="4" t="str">
+        <f>columns!F20</f>
+        <v>date</v>
+      </c>
+      <c r="H20" s="4" t="str">
+        <f>columns!G20</f>
+        <v>帳號創建日期</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>        `dataMemberUsernameMemberText` tinytext NOT NULL COMMENT '使用者名稱',</v>
+      </c>
+      <c r="B21" s="4" t="str">
+        <f>columns!A21</f>
+        <v>dataMemberUsernameMemberText</v>
+      </c>
+      <c r="C21" s="4" t="str">
+        <f>columns!B21</f>
+        <v>Q01</v>
+      </c>
+      <c r="D21" s="4" t="str">
+        <f>columns!C21</f>
+        <v>dataMember</v>
+      </c>
+      <c r="E21" s="4" t="str">
+        <f>columns!D21</f>
+        <v>username</v>
+      </c>
+      <c r="F21" s="4" t="str">
+        <f>columns!E21</f>
+        <v>member</v>
+      </c>
+      <c r="G21" s="4" t="str">
+        <f>columns!F21</f>
+        <v>text</v>
+      </c>
+      <c r="H21" s="4" t="str">
+        <f>columns!G21</f>
+        <v>使用者名稱</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>        `dataMemberPasswordMemberText` tinytext NOT NULL COMMENT '密碼',</v>
+      </c>
+      <c r="B22" s="4" t="str">
+        <f>columns!A22</f>
+        <v>dataMemberPasswordMemberText</v>
+      </c>
+      <c r="C22" s="4" t="str">
+        <f>columns!B22</f>
+        <v>Q02</v>
+      </c>
+      <c r="D22" s="4" t="str">
+        <f>columns!C22</f>
+        <v>dataMember</v>
+      </c>
+      <c r="E22" s="4" t="str">
+        <f>columns!D22</f>
+        <v>password</v>
+      </c>
+      <c r="F22" s="4" t="str">
+        <f>columns!E22</f>
+        <v>member</v>
+      </c>
+      <c r="G22" s="4" t="str">
+        <f>columns!F22</f>
+        <v>text</v>
+      </c>
+      <c r="H22" s="4" t="str">
+        <f>columns!G22</f>
+        <v>密碼</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>        `dataMemberEmailMemberText` tinytext NOT NULL COMMENT '電子郵件'</v>
+      </c>
+      <c r="B23" s="4" t="str">
+        <f>columns!A23</f>
+        <v>dataMemberEmailMemberText</v>
+      </c>
+      <c r="C23" s="4" t="str">
+        <f>columns!B23</f>
+        <v>Q03</v>
+      </c>
+      <c r="D23" s="4" t="str">
+        <f>columns!C23</f>
+        <v>dataMember</v>
+      </c>
+      <c r="E23" s="4" t="str">
+        <f>columns!D23</f>
+        <v>email</v>
+      </c>
+      <c r="F23" s="4" t="str">
+        <f>columns!E23</f>
+        <v>member</v>
+      </c>
+      <c r="G23" s="4" t="str">
+        <f>columns!F23</f>
+        <v>text</v>
+      </c>
+      <c r="H23" s="4" t="str">
+        <f>columns!G23</f>
+        <v>電子郵件</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>    ) ENGINE=InnoDB DEFAULT CHARSET=utf8 COLLATE=utf8_general_ci;</v>
+      </c>
+      <c r="B24" s="4" t="str">
+        <f>columns!A24</f>
+        <v>END</v>
+      </c>
+      <c r="C24" s="4" t="str">
+        <f>columns!B24</f>
+        <v>Z00</v>
+      </c>
+      <c r="D24" s="4" t="str">
+        <f>columns!C24</f>
+        <v>END</v>
+      </c>
+      <c r="E24" s="4" t="str">
+        <f>columns!D24</f>
+        <v/>
+      </c>
+      <c r="F24" s="4" t="str">
+        <f>columns!E24</f>
+        <v/>
+      </c>
+      <c r="G24" s="4" t="str">
+        <f>columns!F24</f>
+        <v/>
+      </c>
+      <c r="H24" s="4" t="str">
+        <f>columns!G24</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="str">
+        <f t="shared" si="1"/>
         <v>EOD ?&gt;</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="1"/>
+      <c r="B25" s="4" t="str">
+        <f>columns!A25</f>
+        <v/>
+      </c>
+      <c r="C25" s="4" t="str">
+        <f>columns!B25</f>
+        <v/>
+      </c>
+      <c r="D25" s="4" t="str">
+        <f>columns!C25</f>
+        <v/>
+      </c>
+      <c r="E25" s="4" t="str">
+        <f>columns!D25</f>
+        <v/>
+      </c>
+      <c r="F25" s="4" t="str">
+        <f>columns!E25</f>
+        <v/>
+      </c>
+      <c r="G25" s="4" t="str">
+        <f>columns!F25</f>
+        <v/>
+      </c>
+      <c r="H25" s="4" t="str">
+        <f>columns!G25</f>
+        <v/>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B26" s="4" t="str">
+        <f>columns!A26</f>
+        <v/>
+      </c>
+      <c r="C26" s="4" t="str">
+        <f>columns!B26</f>
+        <v/>
+      </c>
+      <c r="D26" s="4" t="str">
+        <f>columns!C26</f>
+        <v/>
+      </c>
+      <c r="E26" s="4" t="str">
+        <f>columns!D26</f>
+        <v/>
+      </c>
+      <c r="F26" s="4" t="str">
+        <f>columns!E26</f>
+        <v/>
+      </c>
+      <c r="G26" s="4" t="str">
+        <f>columns!F26</f>
+        <v/>
+      </c>
+      <c r="H26" s="4" t="str">
+        <f>columns!G26</f>
+        <v/>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1"/>
@@ -2825,11 +3463,11 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="3" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="7" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="H1" s="7"/>
       <c r="I1" s="5"/>
@@ -2857,28 +3495,28 @@
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="3" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -2911,15 +3549,15 @@
         <v>[language=Chinese] [i18n=header]:before{content:"請領（補發、換發）記帳士證書申請書"}[language=Chinese] [i18n=header]:after{content:""}[language=English] [i18n=header]:before{content:"Application Form for The Issuance (Reissuance, Replacement) of Certificate of Public Bookkeeper"}[language=English] [i18n=header]:after{content:""}</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="8" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="7" t="str">
-        <f t="shared" ref="G3:G36" si="2">if(H3="", ""
+        <f t="shared" ref="G3:G34" si="2">if(H3="", ""
 ,if(I3&lt;&gt;"", I3, H3))</f>
         <v>Application Form for The Issuance (Reissuance, Replacement) of Certificate of Public Bookkeeper</v>
       </c>
@@ -2928,7 +3566,7 @@
         <v>Please lead (replenishment, renewal) bookkeeper certificate application</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -2957,11 +3595,11 @@
         <v>[language=Chinese] [i18n=dateOfApplication]:before{content:"申請日期："}[language=Chinese] [i18n=dateOfApplication]:after{content:""}[language=English] [i18n=dateOfApplication]:before{content:"Date of Application: "}[language=English] [i18n=dateOfApplication]:after{content:""}</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="8" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="7" t="str">
@@ -2973,7 +3611,7 @@
         <v>Date of Application:</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -3002,11 +3640,11 @@
         <v>[language=Chinese] [i18n=recipient]:before{content:"受文者："}[language=Chinese] [i18n=recipient]:after{content:""}[language=English] [i18n=recipient]:before{content:"Recipient:"}[language=English] [i18n=recipient]:after{content:""}</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="8" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="7" t="str">
@@ -3018,7 +3656,7 @@
         <v>Writer:</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -3047,11 +3685,11 @@
         <v>[language=Chinese] [i18n=ministryOfFinance]:before{content:"財政部"}[language=Chinese] [i18n=ministryOfFinance]:after{content:""}[language=English] [i18n=ministryOfFinance]:before{content:"Ministry of Finance"}[language=English] [i18n=ministryOfFinance]:after{content:""}</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="8" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="7" t="str">
@@ -3063,7 +3701,7 @@
         <v>Ministry of Finance</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -3092,11 +3730,11 @@
         <v>[language=Chinese] [i18n=purpose]:before{content:"主旨："}[language=Chinese] [i18n=purpose]:after{content:""}[language=English] [i18n=purpose]:before{content:"Purpose:"}[language=English] [i18n=purpose]:after{content:""}</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="8" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="7" t="str">
@@ -3108,7 +3746,7 @@
         <v>Theme:</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -3137,11 +3775,11 @@
         <v>[language=Chinese] [i18n=toApplyFor]:before{content:"申請"}[language=Chinese] [i18n=toApplyFor]:after{content:""}[language=English] [i18n=toApplyFor]:before{content:"To apply for"}[language=English] [i18n=toApplyFor]:after{content:""}</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="7" t="str">
@@ -3153,7 +3791,7 @@
         <v>Apply</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -3182,11 +3820,11 @@
         <v>[language=Chinese] [i18n=description]:before{content:"說明："}[language=Chinese] [i18n=description]:after{content:""}[language=English] [i18n=description]:before{content:"Description:"}[language=English] [i18n=description]:after{content:""}</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="7" t="str">
@@ -3198,7 +3836,7 @@
         <v>illustrate:</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -3227,11 +3865,11 @@
         <v>[language=Chinese] [i18n=descriptionA]:before{content:"一、依記帳士法第 5 條暨記帳士證書核發辦法規定辦理。"}[language=Chinese] [i18n=descriptionA]:after{content:""}[language=English] [i18n=descriptionA]:before{content:"1. Handled in accordance with Article 5 of the Certified Public Bookkeepers Act and Rules Governing Issuance of Certificate of Public Bookkeeper."}[language=English] [i18n=descriptionA]:after{content:""}</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="7" t="str">
@@ -3243,7 +3881,7 @@
         <v>1. According to Article 5 of the Account Law and the Account Certificate, the method of issuance of the accounting certificate shall be handled.</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -3272,11 +3910,11 @@
         <v>[language=Chinese] [i18n=descriptionB]:before{content:"二、茲檢具下列文件：（請勾選檢附項目，詳註二）。"}[language=Chinese] [i18n=descriptionB]:after{content:""}[language=English] [i18n=descriptionB]:before{content:"2. The following documents are hereby inspected: (Please tick the attached items, see Note 2)."}[language=English] [i18n=descriptionB]:after{content:""}</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="7" t="str">
@@ -3288,7 +3926,7 @@
         <v>Second, the following documents: (Please check the attachment project, detailed note 2).</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -3317,11 +3955,11 @@
         <v>[language=Chinese] [i18n=descriptionBA]:before{content:"（一）記帳士考試及格證書正本及影本各 1 份；記帳士考試及格證書為電子證書型式者，為其列印本 1 份。"}[language=Chinese] [i18n=descriptionBA]:after{content:""}[language=English] [i18n=descriptionBA]:before{content:"a. The original and a photocopy of the certificate for passing the certified public bookkeepers examination; if the certificate for passing the certified public bookkeepers examination is of the electronic certificate type, the applicant shall attach a printout of the certificate."}[language=English] [i18n=descriptionBA]:after{content:""}</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="7" t="str">
@@ -3333,7 +3971,7 @@
         <v>(1) The original and one copy of the book test and a certificate; the bookkeeper test and the certificate of the certificate are the electronic certificate type, and one copy of them.</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -3362,11 +4000,11 @@
         <v>[language=Chinese] [i18n=descriptionBB]:before{content:"（二）履歷表一份。"}[language=Chinese] [i18n=descriptionBB]:after{content:""}[language=English] [i18n=descriptionBB]:before{content:"b. A curriculum vitae of the applicant."}[language=English] [i18n=descriptionBB]:after{content:""}</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="7" t="str">
@@ -3378,7 +4016,7 @@
         <v>(2) A resume.</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -3407,11 +4045,11 @@
         <v>[language=Chinese] [i18n=descriptionBC]:before{content:"（三）國民身分證正反面影本 1 份（如範例），外國人為護照、外僑居留證或永久居留證影本。"}[language=Chinese] [i18n=descriptionBC]:after{content:""}[language=English] [i18n=descriptionBC]:before{content:"c. A photocopy of the front and back of the identification card of the applicant (See example), a photocopy of the passport, Alien Resident Certificate, or Alien Permanent Resident Certificate of the foreign applicant."}[language=English] [i18n=descriptionBC]:after{content:""}</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="7" t="str">
@@ -3423,7 +4061,7 @@
         <v>(3) One copy of the national identity card (such as examples), foreigners are passports, foreigners' residence permits or permanent residence permits.</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
@@ -3452,11 +4090,11 @@
         <v>[language=Chinese] [i18n=descriptionBD]:before{content:"（四）最近 1 年內 2 吋半身相片 2 張（詳註三）。"}[language=Chinese] [i18n=descriptionBD]:after{content:""}[language=English] [i18n=descriptionBD]:before{content:"d. Two 2-inch photographs of the applicant taken within the year (Note 3)."}[language=English] [i18n=descriptionBD]:after{content:""}</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="7" t="str">
@@ -3468,7 +4106,7 @@
         <v>(4) Two 2 -inch half -body photos in the past year (details 3).</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -3497,11 +4135,11 @@
         <v>[language=Chinese] [i18n=descriptionBE]:before{content:"（五）證書費新臺幣壹仟伍佰元整（詳註四）。"}[language=Chinese] [i18n=descriptionBE]:after{content:""}[language=English] [i18n=descriptionBE]:before{content:"e. The amount of the certification fee payable is NT$1,500 (Note 4)."}[language=English] [i18n=descriptionBE]:after{content:""}</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="7" t="str">
@@ -3513,7 +4151,7 @@
         <v>(5) NT $ 1 of Certificate Fee Tong (Detailed Note 4).</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -3542,11 +4180,11 @@
         <v>[language=Chinese] [i18n=descriptionBF]:before{content:"（六）原撤銷或廢止原因消滅之證明文件。"}[language=Chinese] [i18n=descriptionBF]:after{content:""}[language=English] [i18n=descriptionBF]:before{content:"f. Documentary evidence that the reason for the revocation or cancellation of the original certificate has ceased to exist."}[language=English] [i18n=descriptionBF]:after{content:""}</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="7" t="str">
@@ -3558,7 +4196,7 @@
         <v>(6) The document of the destruction of the cause of the reasons for dismissal.</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
@@ -3587,11 +4225,11 @@
         <v>[language=Chinese] [i18n=descriptionBG]:before{content:"（七）記帳士證書遺失或滅失登報 3 天聲明作廢之整張報紙。"}[language=Chinese] [i18n=descriptionBG]:after{content:""}[language=English] [i18n=descriptionBG]:before{content:"g. The whole page of the newspaper in which the notice of nullification of certificate of public bookkeeper due to loss or destruction thereof is published for three (3) days."}[language=English] [i18n=descriptionBG]:after{content:""}</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="7" t="str">
@@ -3603,7 +4241,7 @@
         <v>(7) The entire newspaper of the losses or loss of the bookkeeper's certificate is lost for 3 days.</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -3632,11 +4270,11 @@
         <v>[language=Chinese] [i18n=descriptionBH]:before{content:"（八）污損、破損或更名前之記帳士證書。"}[language=Chinese] [i18n=descriptionBH]:after{content:""}[language=English] [i18n=descriptionBH]:before{content:"h. The stained, damaged or pre-name Certified Public bookkeeper’s certificate."}[language=English] [i18n=descriptionBH]:after{content:""}</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="7" t="str">
@@ -3648,7 +4286,7 @@
         <v>(8) Discovery, damage, or renamed account certificate certificate.</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
@@ -3677,11 +4315,11 @@
         <v>[language=Chinese] [i18n=descriptionBI]:before{content:"（九）中文版記帳士證書及有效護照影本各 1  份。"}[language=Chinese] [i18n=descriptionBI]:after{content:""}[language=English] [i18n=descriptionBI]:before{content:"i. The Chinese Version of the Certificate of Public Bookkeeper and the valid passport of the applicant, with a photocopy of each."}[language=English] [i18n=descriptionBI]:after{content:""}</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="7" t="str">
@@ -3693,7 +4331,7 @@
         <v>(9) The Chinese version of the bookkeeping certificate and the valid passport shadow.</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
@@ -3722,11 +4360,11 @@
         <v>[language=Chinese] [i18n=descriptionC]:before{content:"三、聲明事項："}[language=Chinese] [i18n=descriptionC]:after{content:""}[language=English] [i18n=descriptionC]:before{content:"3. Disclaimer:"}[language=English] [i18n=descriptionC]:after{content:""}</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="7" t="str">
@@ -3738,7 +4376,7 @@
         <v>3. Declaration matters:</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -3767,11 +4405,11 @@
         <v>[language=Chinese] [i18n=descriptionCA]:before{content:"（一）申請人確無記帳士法第 4 條第 1 項各款不得充任記帳士情事。"}[language=Chinese] [i18n=descriptionCA]:after{content:""}[language=English] [i18n=descriptionCA]:before{content:"a. The applicant does not have the conditions under Subparagraph 1, Article 4 of the Certified Public Bookkeepers Act that he/she shall not act as a certified public bookkeeper."}[language=English] [i18n=descriptionCA]:after{content:""}</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="7" t="str">
@@ -3783,7 +4421,7 @@
         <v>(1) The applicant does not have the book 4 (1), paragraph 1, paragraph 1 of each account.</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -3812,11 +4450,11 @@
         <v>[language=Chinese] [i18n=descriptionCB]:before{content:"（二）申請人所填資料及附繳文件均為真實，如有不實願負法律責任。"}[language=Chinese] [i18n=descriptionCB]:after{content:""}[language=English] [i18n=descriptionCB]:before{content:"b. The information filled in by the applicant and the attached documents are all true; if there is any untrue statement, the applicant accepts the legal responsibility."}[language=English] [i18n=descriptionCB]:after{content:""}</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="7" t="str">
@@ -3828,7 +4466,7 @@
         <v>(2) The information filled by the applicant and the attachment documents are true, and if they are unreasonable, they are unwilling to bear legal responsibility.</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -3857,11 +4495,11 @@
         <v>[language=Chinese] [i18n=applicantInformation]:before{content:"申請人資料："}[language=Chinese] [i18n=applicantInformation]:after{content:""}[language=English] [i18n=applicantInformation]:before{content:"Applicant information:"}[language=English] [i18n=applicantInformation]:after{content:""}</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="7" t="str">
@@ -3873,7 +4511,7 @@
         <v>Applicant information:</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -3902,13 +4540,13 @@
         <v>[language=Chinese] [i18n=applyFor]:before{content:"申請項目"}[language=Chinese] [i18n=applyFor]:after{content:""}[language=English] [i18n=applyFor]:before{content:"Apply for"}[language=English] [i18n=applyFor]:after{content:""}</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="7" t="str">
@@ -3920,7 +4558,7 @@
         <v>Application Project</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -3949,13 +4587,13 @@
         <v>[language=Chinese] [i18n=applicant]:before{content:"申請人"}[language=Chinese] [i18n=applicant]:after{content:""}[language=English] [i18n=applicant]:before{content:"Applicant"}[language=English] [i18n=applicant]:after{content:""}</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="7" t="str">
@@ -3967,7 +4605,7 @@
         <v>applicant</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -3996,13 +4634,13 @@
         <v>[language=Chinese] [i18n=identityCardNumber]:before{content:"身分證字號"}[language=Chinese] [i18n=identityCardNumber]:after{content:""}[language=English] [i18n=identityCardNumber]:before{content:"ID number"}[language=English] [i18n=identityCardNumber]:after{content:""}</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="7" t="str">
@@ -4014,7 +4652,7 @@
         <v>ID number</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -4043,13 +4681,13 @@
         <v>[language=Chinese] [i18n=contactNumber]:before{content:"連絡電話"}[language=Chinese] [i18n=contactNumber]:after{content:""}[language=English] [i18n=contactNumber]:before{content:"Contact number"}[language=English] [i18n=contactNumber]:after{content:""}</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="7" t="str">
@@ -4061,7 +4699,7 @@
         <v>Connection</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -4090,13 +4728,13 @@
         <v>[language=Chinese] [i18n=phoneNumber]:before{content:"手機號碼"}[language=Chinese] [i18n=phoneNumber]:after{content:""}[language=English] [i18n=phoneNumber]:before{content:"Phone number"}[language=English] [i18n=phoneNumber]:after{content:""}</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="7" t="str">
@@ -4108,7 +4746,7 @@
         <v>phone number</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -4137,13 +4775,13 @@
         <v>[language=Chinese] [i18n=residence]:before{content:"居住縣市"}[language=Chinese] [i18n=residence]:after{content:""}[language=English] [i18n=residence]:before{content:"City/County of residence"}[language=English] [i18n=residence]:after{content:""}</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="7" t="str">
@@ -4155,7 +4793,7 @@
         <v>Residential county</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -4184,13 +4822,13 @@
         <v>[language=Chinese] [i18n=address]:before{content:"通訊地址"}[language=Chinese] [i18n=address]:after{content:""}[language=English] [i18n=address]:before{content:"Address"}[language=English] [i18n=address]:after{content:""}</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="7" t="str">
@@ -4202,7 +4840,7 @@
         <v>mailing address</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -4227,24 +4865,35 @@
     <row r="32">
       <c r="A32" s="5"/>
       <c r="B32" s="7" t="str">
-        <f t="shared" ref="B32:B36" si="3">if(C32="", "",
+        <f t="shared" ref="B32:B34" si="3">if(C32="", "",
 "[lang=Chinese] [i18n="&amp;C32&amp;"]:before{content:"""&amp;E32&amp;"""}"
 &amp;"[lang=Chinese] [i18n="&amp;C32&amp;"]:after{content:"""&amp;F32&amp;"""}"
 &amp;"[lang=English] [i18n="&amp;C32&amp;"]:before{content:"""&amp;G32&amp;"""}"
 &amp;"[lang=English] [i18n="&amp;C32&amp;"]:after{content:"""&amp;J32&amp;"""}"
 )</f>
-        <v/>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
+        <v>[lang=Chinese] [i18n=username]:before{content:"使用者名稱"}[lang=Chinese] [i18n=username]:after{content:""}[lang=English] [i18n=username]:before{content:"Username"}[lang=English] [i18n=username]:after{content:""}</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="F32" s="5"/>
       <c r="G32" s="7" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="H32" s="6"/>
-      <c r="I32" s="5"/>
+        <v>Username</v>
+      </c>
+      <c r="H32" s="7" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("iferror(GOOGLETRANSLATE(E32,""zh-tw"",""en""),"""")"),"username")</f>
+        <v>username</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>146</v>
+      </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
@@ -4269,18 +4918,29 @@
       <c r="A33" s="5"/>
       <c r="B33" s="7" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+        <v>[lang=Chinese] [i18n=password]:before{content:"密碼"}[lang=Chinese] [i18n=password]:after{content:""}[lang=English] [i18n=password]:before{content:"Password"}[lang=English] [i18n=password]:after{content:""}</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="F33" s="5"/>
       <c r="G33" s="7" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="H33" s="6"/>
-      <c r="I33" s="5"/>
+        <v>Password</v>
+      </c>
+      <c r="H33" s="7" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("iferror(GOOGLETRANSLATE(E33,""zh-tw"",""en""),"""")"),"password")</f>
+        <v>password</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>148</v>
+      </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
@@ -4305,18 +4965,29 @@
       <c r="A34" s="5"/>
       <c r="B34" s="7" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
+        <v>[lang=Chinese] [i18n=email]:before{content:"電子郵件"}[lang=Chinese] [i18n=email]:after{content:""}[lang=English] [i18n=email]:before{content:"Email"}[lang=English] [i18n=email]:after{content:""}</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="F34" s="5"/>
       <c r="G34" s="7" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="H34" s="6"/>
-      <c r="I34" s="5"/>
+        <v>Email</v>
+      </c>
+      <c r="H34" s="7" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("iferror(GOOGLETRANSLATE(E34,""zh-tw"",""en""),"""")"),"e-mail")</f>
+        <v>e-mail</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
@@ -4339,18 +5010,12 @@
     </row>
     <row r="35">
       <c r="A35" s="5"/>
-      <c r="B35" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="B35" s="6"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
@@ -4375,18 +5040,12 @@
     </row>
     <row r="36">
       <c r="A36" s="5"/>
-      <c r="B36" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="B36" s="6"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
@@ -9239,96 +9898,6 @@
       <c r="AA197" s="5"/>
       <c r="AB197" s="5"/>
     </row>
-    <row r="198">
-      <c r="A198" s="5"/>
-      <c r="B198" s="6"/>
-      <c r="C198" s="5"/>
-      <c r="D198" s="5"/>
-      <c r="E198" s="5"/>
-      <c r="F198" s="5"/>
-      <c r="G198" s="6"/>
-      <c r="H198" s="6"/>
-      <c r="I198" s="5"/>
-      <c r="J198" s="5"/>
-      <c r="K198" s="5"/>
-      <c r="L198" s="5"/>
-      <c r="M198" s="5"/>
-      <c r="N198" s="5"/>
-      <c r="O198" s="5"/>
-      <c r="P198" s="5"/>
-      <c r="Q198" s="5"/>
-      <c r="R198" s="5"/>
-      <c r="S198" s="5"/>
-      <c r="T198" s="5"/>
-      <c r="U198" s="5"/>
-      <c r="V198" s="5"/>
-      <c r="W198" s="5"/>
-      <c r="X198" s="5"/>
-      <c r="Y198" s="5"/>
-      <c r="Z198" s="5"/>
-      <c r="AA198" s="5"/>
-      <c r="AB198" s="5"/>
-    </row>
-    <row r="199">
-      <c r="A199" s="5"/>
-      <c r="B199" s="6"/>
-      <c r="C199" s="5"/>
-      <c r="D199" s="5"/>
-      <c r="E199" s="5"/>
-      <c r="F199" s="5"/>
-      <c r="G199" s="6"/>
-      <c r="H199" s="6"/>
-      <c r="I199" s="5"/>
-      <c r="J199" s="5"/>
-      <c r="K199" s="5"/>
-      <c r="L199" s="5"/>
-      <c r="M199" s="5"/>
-      <c r="N199" s="5"/>
-      <c r="O199" s="5"/>
-      <c r="P199" s="5"/>
-      <c r="Q199" s="5"/>
-      <c r="R199" s="5"/>
-      <c r="S199" s="5"/>
-      <c r="T199" s="5"/>
-      <c r="U199" s="5"/>
-      <c r="V199" s="5"/>
-      <c r="W199" s="5"/>
-      <c r="X199" s="5"/>
-      <c r="Y199" s="5"/>
-      <c r="Z199" s="5"/>
-      <c r="AA199" s="5"/>
-      <c r="AB199" s="5"/>
-    </row>
-    <row r="200">
-      <c r="A200" s="5"/>
-      <c r="B200" s="6"/>
-      <c r="C200" s="5"/>
-      <c r="D200" s="5"/>
-      <c r="E200" s="5"/>
-      <c r="F200" s="5"/>
-      <c r="G200" s="6"/>
-      <c r="H200" s="6"/>
-      <c r="I200" s="5"/>
-      <c r="J200" s="5"/>
-      <c r="K200" s="5"/>
-      <c r="L200" s="5"/>
-      <c r="M200" s="5"/>
-      <c r="N200" s="5"/>
-      <c r="O200" s="5"/>
-      <c r="P200" s="5"/>
-      <c r="Q200" s="5"/>
-      <c r="R200" s="5"/>
-      <c r="S200" s="5"/>
-      <c r="T200" s="5"/>
-      <c r="U200" s="5"/>
-      <c r="V200" s="5"/>
-      <c r="W200" s="5"/>
-      <c r="X200" s="5"/>
-      <c r="Y200" s="5"/>
-      <c r="Z200" s="5"/>
-      <c r="AA200" s="5"/>
-      <c r="AB200" s="5"/>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -9353,10 +9922,10 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="3" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="5"/>
@@ -9383,22 +9952,22 @@
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="3" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -9430,13 +9999,13 @@
         <v>[language=Chinese] [select=true][i18n=firstTime]:before{content:"☑第1次請領"}[language=Chinese] [select=false][i18n=firstTime]:before{content:"☐第1次請領"}[language=English] [select=true][i18n=firstTime]:before{content:"☑Issuance for the first time"}[language=English] [select=false][i18n=firstTime]:before{content:"☐Issuance for the first time"}</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="F3" s="7" t="str">
         <f t="shared" ref="F3:F29" si="2">if(H3&lt;&gt;"",H3,G3)</f>
@@ -9447,7 +10016,7 @@
         <v>The first time, please lead</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -9475,13 +10044,13 @@
         <v>[language=Chinese] [select=true][i18n=certificateHasCeased]:before{content:"☑撤銷原因消滅補發"}[language=Chinese] [select=false][i18n=certificateHasCeased]:before{content:"☐撤銷原因消滅補發"}[language=English] [select=true][i18n=certificateHasCeased]:before{content:"☑Reissuance due to the reason for the revocation or cancellation of the original certificate has ceased to exist"}[language=English] [select=false][i18n=certificateHasCeased]:before{content:"☐Reissuance due to the reason for the revocation or cancellation of the original certificate has ceased to exist"}</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="F4" s="7" t="str">
         <f t="shared" si="2"/>
@@ -9492,7 +10061,7 @@
         <v>Rejuvenation reasons to eliminate replenishment</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -9520,13 +10089,13 @@
         <v>[language=Chinese] [select=true][i18n=lost]:before{content:"☑遺失補發"}[language=Chinese] [select=false][i18n=lost]:before{content:"☐遺失補發"}[language=English] [select=true][i18n=lost]:before{content:"☑Reissuance for lost certificate"}[language=English] [select=false][i18n=lost]:before{content:"☐Reissuance for lost certificate"}</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="F5" s="7" t="str">
         <f t="shared" si="2"/>
@@ -9537,7 +10106,7 @@
         <v>Loss of replenishment</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -9565,13 +10134,13 @@
         <v>[language=Chinese] [select=true][i18n=replacement]:before{content:"☑換發記帳士證書"}[language=Chinese] [select=false][i18n=replacement]:before{content:"☐換發記帳士證書"}[language=English] [select=true][i18n=replacement]:before{content:"☑Replacement of the Certificate of Public Bookkeeper"}[language=English] [select=false][i18n=replacement]:before{content:"☐Replacement of the Certificate of Public Bookkeeper"}</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="F6" s="7" t="str">
         <f t="shared" si="2"/>
@@ -9582,7 +10151,7 @@
         <v>Removal account certificate certificate</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -9610,13 +10179,13 @@
         <v>[language=Chinese] [select=true][i18n=englishVersion]:before{content:"☑英文版記帳士證書"}[language=Chinese] [select=false][i18n=englishVersion]:before{content:"☐英文版記帳士證書"}[language=English] [select=true][i18n=englishVersion]:before{content:"☑The English Version of the Certificate of Public Bookkeeper"}[language=English] [select=false][i18n=englishVersion]:before{content:"☐The English Version of the Certificate of Public Bookkeeper"}</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="F7" s="7" t="str">
         <f t="shared" si="2"/>
@@ -9627,7 +10196,7 @@
         <v>English version of the bookkeeper certificate</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -9655,14 +10224,14 @@
         <v>[language=Chinese] [select=true][i18n=taipeiCity]:before{content:"☑台北市"}[language=Chinese] [select=false][i18n=taipeiCity]:before{content:"☐台北市"}[language=English] [select=true][i18n=taipeiCity]:before{content:"☑Taipei City"}[language=English] [select=false][i18n=taipeiCity]:before{content:"☐Taipei City"}</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" ref="D8:D29" si="3">"dataForm" &amp; replace(C8,1,1, UPPER(LEFT(C8,1)))</f>
         <v>dataFormTaipeiCity</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="F8" s="7" t="str">
         <f t="shared" si="2"/>
@@ -9673,7 +10242,7 @@
         <v>Taipei City</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -9701,14 +10270,14 @@
         <v>[language=Chinese] [select=true][i18n=keelungCity]:before{content:"☑基隆市"}[language=Chinese] [select=false][i18n=keelungCity]:before{content:"☐基隆市"}[language=English] [select=true][i18n=keelungCity]:before{content:"☑Keelung City"}[language=English] [select=false][i18n=keelungCity]:before{content:"☐Keelung City"}</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormKeelungCity</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="F9" s="7" t="str">
         <f t="shared" si="2"/>
@@ -9719,7 +10288,7 @@
         <v>Keelung City</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -9747,14 +10316,14 @@
         <v>[language=Chinese] [select=true][i18n=newTaipeiCity]:before{content:"☑新北市"}[language=Chinese] [select=false][i18n=newTaipeiCity]:before{content:"☐新北市"}[language=English] [select=true][i18n=newTaipeiCity]:before{content:"☑New Taipei City"}[language=English] [select=false][i18n=newTaipeiCity]:before{content:"☐New Taipei City"}</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormNewTaipeiCity</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="F10" s="7" t="str">
         <f t="shared" si="2"/>
@@ -9765,7 +10334,7 @@
         <v>New Taipei City</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -9793,14 +10362,14 @@
         <v>[language=Chinese] [select=true][i18n=lienchiangCounty]:before{content:"☑連江縣"}[language=Chinese] [select=false][i18n=lienchiangCounty]:before{content:"☐連江縣"}[language=English] [select=true][i18n=lienchiangCounty]:before{content:"☑Lienchiang County"}[language=English] [select=false][i18n=lienchiangCounty]:before{content:"☐Lienchiang County"}</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormLienchiangCounty</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="F11" s="7" t="str">
         <f t="shared" si="2"/>
@@ -9811,7 +10380,7 @@
         <v>Lianjiang County</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -9839,14 +10408,14 @@
         <v>[language=Chinese] [select=true][i18n=yilanCounty]:before{content:"☑宜蘭縣"}[language=Chinese] [select=false][i18n=yilanCounty]:before{content:"☐宜蘭縣"}[language=English] [select=true][i18n=yilanCounty]:before{content:"☑Yilan County"}[language=English] [select=false][i18n=yilanCounty]:before{content:"☐Yilan County"}</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormYilanCounty</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
       <c r="F12" s="7" t="str">
         <f t="shared" si="2"/>
@@ -9857,7 +10426,7 @@
         <v>Yilan County</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -9885,14 +10454,14 @@
         <v>[language=Chinese] [select=true][i18n=hsinchuCity]:before{content:"☑新竹市"}[language=Chinese] [select=false][i18n=hsinchuCity]:before{content:"☐新竹市"}[language=English] [select=true][i18n=hsinchuCity]:before{content:"☑Hsinchu City"}[language=English] [select=false][i18n=hsinchuCity]:before{content:"☐Hsinchu City"}</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormHsinchuCity</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
       <c r="F13" s="7" t="str">
         <f t="shared" si="2"/>
@@ -9903,7 +10472,7 @@
         <v>Hsinchu City</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -9931,14 +10500,14 @@
         <v>[language=Chinese] [select=true][i18n=hsinchuCounty]:before{content:"☑新竹縣"}[language=Chinese] [select=false][i18n=hsinchuCounty]:before{content:"☐新竹縣"}[language=English] [select=true][i18n=hsinchuCounty]:before{content:"☑Hsinchu County"}[language=English] [select=false][i18n=hsinchuCounty]:before{content:"☐Hsinchu County"}</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormHsinchuCounty</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
       <c r="F14" s="7" t="str">
         <f t="shared" si="2"/>
@@ -9949,7 +10518,7 @@
         <v>Hsinchu County</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>166</v>
+        <v>191</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -9977,14 +10546,14 @@
         <v>[language=Chinese] [select=true][i18n=taoyuanCity]:before{content:"☑桃園市"}[language=Chinese] [select=false][i18n=taoyuanCity]:before{content:"☐桃園市"}[language=English] [select=true][i18n=taoyuanCity]:before{content:"☑Taoyuan City"}[language=English] [select=false][i18n=taoyuanCity]:before{content:"☐Taoyuan City"}</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormTaoyuanCity</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="F15" s="7" t="str">
         <f t="shared" si="2"/>
@@ -9995,7 +10564,7 @@
         <v>Taoyuan City</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -10023,14 +10592,14 @@
         <v>[language=Chinese] [select=true][i18n=miaoliCounty]:before{content:"☑苗栗縣"}[language=Chinese] [select=false][i18n=miaoliCounty]:before{content:"☐苗栗縣"}[language=English] [select=true][i18n=miaoliCounty]:before{content:"☑Miaoli County"}[language=English] [select=false][i18n=miaoliCounty]:before{content:"☐Miaoli County"}</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormMiaoliCounty</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="F16" s="7" t="str">
         <f t="shared" si="2"/>
@@ -10041,7 +10610,7 @@
         <v>Miaoli County</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>172</v>
+        <v>197</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -10069,14 +10638,14 @@
         <v>[language=Chinese] [select=true][i18n=taichungCity]:before{content:"☑台中市"}[language=Chinese] [select=false][i18n=taichungCity]:before{content:"☐台中市"}[language=English] [select=true][i18n=taichungCity]:before{content:"☑Taichung City"}[language=English] [select=false][i18n=taichungCity]:before{content:"☐Taichung City"}</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormTaichungCity</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="F17" s="7" t="str">
         <f t="shared" si="2"/>
@@ -10087,7 +10656,7 @@
         <v>Taichung City</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -10115,14 +10684,14 @@
         <v>[language=Chinese] [select=true][i18n=changhuaCounty]:before{content:"☑彰化縣"}[language=Chinese] [select=false][i18n=changhuaCounty]:before{content:"☐彰化縣"}[language=English] [select=true][i18n=changhuaCounty]:before{content:"☑Changhua County"}[language=English] [select=false][i18n=changhuaCounty]:before{content:"☐Changhua County"}</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormChanghuaCounty</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="F18" s="7" t="str">
         <f t="shared" si="2"/>
@@ -10133,7 +10702,7 @@
         <v>Changhua County</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -10161,14 +10730,14 @@
         <v>[language=Chinese] [select=true][i18n=nantouCounty]:before{content:"☑南投縣"}[language=Chinese] [select=false][i18n=nantouCounty]:before{content:"☐南投縣"}[language=English] [select=true][i18n=nantouCounty]:before{content:"☑Nantou County"}[language=English] [select=false][i18n=nantouCounty]:before{content:"☐Nantou County"}</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormNantouCounty</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="F19" s="7" t="str">
         <f t="shared" si="2"/>
@@ -10179,7 +10748,7 @@
         <v>Nantou County</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>181</v>
+        <v>206</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -10207,14 +10776,14 @@
         <v>[language=Chinese] [select=true][i18n=chiayiCity]:before{content:"☑嘉義市"}[language=Chinese] [select=false][i18n=chiayiCity]:before{content:"☐嘉義市"}[language=English] [select=true][i18n=chiayiCity]:before{content:"☑Chiayi City"}[language=English] [select=false][i18n=chiayiCity]:before{content:"☐Chiayi City"}</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="D20" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormChiayiCity</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="F20" s="7" t="str">
         <f t="shared" si="2"/>
@@ -10225,7 +10794,7 @@
         <v>Chiayi City</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>184</v>
+        <v>209</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -10253,14 +10822,14 @@
         <v>[language=Chinese] [select=true][i18n=chiayiCounty]:before{content:"☑嘉義縣"}[language=Chinese] [select=false][i18n=chiayiCounty]:before{content:"☐嘉義縣"}[language=English] [select=true][i18n=chiayiCounty]:before{content:"☑Chiayi County"}[language=English] [select=false][i18n=chiayiCounty]:before{content:"☐Chiayi County"}</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormChiayiCounty</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="F21" s="7" t="str">
         <f t="shared" si="2"/>
@@ -10271,7 +10840,7 @@
         <v>Chiayi County</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -10299,14 +10868,14 @@
         <v>[language=Chinese] [select=true][i18n=yunlinCounty]:before{content:"☑雲林縣"}[language=Chinese] [select=false][i18n=yunlinCounty]:before{content:"☐雲林縣"}[language=English] [select=true][i18n=yunlinCounty]:before{content:"☑Yunlin County"}[language=English] [select=false][i18n=yunlinCounty]:before{content:"☐Yunlin County"}</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormYunlinCounty</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="F22" s="7" t="str">
         <f t="shared" si="2"/>
@@ -10317,7 +10886,7 @@
         <v>Yunlin County</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>190</v>
+        <v>215</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -10345,14 +10914,14 @@
         <v>[language=Chinese] [select=true][i18n=tainanCity]:before{content:"☑台南市"}[language=Chinese] [select=false][i18n=tainanCity]:before{content:"☐台南市"}[language=English] [select=true][i18n=tainanCity]:before{content:"☑Tainan City"}[language=English] [select=false][i18n=tainanCity]:before{content:"☐Tainan City"}</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormTainanCity</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>192</v>
+        <v>217</v>
       </c>
       <c r="F23" s="7" t="str">
         <f t="shared" si="2"/>
@@ -10363,7 +10932,7 @@
         <v>Tainan City</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>193</v>
+        <v>218</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -10391,14 +10960,14 @@
         <v>[language=Chinese] [select=true][i18n=kaohsiungCity]:before{content:"☑高雄市"}[language=Chinese] [select=false][i18n=kaohsiungCity]:before{content:"☐高雄市"}[language=English] [select=true][i18n=kaohsiungCity]:before{content:"☑Kaohsiung City"}[language=English] [select=false][i18n=kaohsiungCity]:before{content:"☐Kaohsiung City"}</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>194</v>
+        <v>219</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormKaohsiungCity</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>195</v>
+        <v>220</v>
       </c>
       <c r="F24" s="7" t="str">
         <f t="shared" si="2"/>
@@ -10409,7 +10978,7 @@
         <v>Kaohsiung</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>196</v>
+        <v>221</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
@@ -10437,14 +11006,14 @@
         <v>[language=Chinese] [select=true][i18n=penghuCounty]:before{content:"☑澎湖縣"}[language=Chinese] [select=false][i18n=penghuCounty]:before{content:"☐澎湖縣"}[language=English] [select=true][i18n=penghuCounty]:before{content:"☑Penghu County"}[language=English] [select=false][i18n=penghuCounty]:before{content:"☐Penghu County"}</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>197</v>
+        <v>222</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormPenghuCounty</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="F25" s="7" t="str">
         <f t="shared" si="2"/>
@@ -10455,7 +11024,7 @@
         <v>Penghu County</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>199</v>
+        <v>224</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
@@ -10483,14 +11052,14 @@
         <v>[language=Chinese] [select=true][i18n=kinmenCounty]:before{content:"☑金門縣"}[language=Chinese] [select=false][i18n=kinmenCounty]:before{content:"☐金門縣"}[language=English] [select=true][i18n=kinmenCounty]:before{content:"☑Kinmen County"}[language=English] [select=false][i18n=kinmenCounty]:before{content:"☐Kinmen County"}</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormKinmenCounty</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>201</v>
+        <v>226</v>
       </c>
       <c r="F26" s="7" t="str">
         <f t="shared" si="2"/>
@@ -10501,7 +11070,7 @@
         <v>Kinmen County</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>202</v>
+        <v>227</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
@@ -10529,14 +11098,14 @@
         <v>[language=Chinese] [select=true][i18n=pingtungCounty]:before{content:"☑屏東縣"}[language=Chinese] [select=false][i18n=pingtungCounty]:before{content:"☐屏東縣"}[language=English] [select=true][i18n=pingtungCounty]:before{content:"☑Pingtung County"}[language=English] [select=false][i18n=pingtungCounty]:before{content:"☐Pingtung County"}</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>203</v>
+        <v>228</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormPingtungCounty</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>204</v>
+        <v>229</v>
       </c>
       <c r="F27" s="7" t="str">
         <f t="shared" si="2"/>
@@ -10547,7 +11116,7 @@
         <v>Pingtung County</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
@@ -10575,14 +11144,14 @@
         <v>[language=Chinese] [select=true][i18n=taitungCounty]:before{content:"☑台東縣"}[language=Chinese] [select=false][i18n=taitungCounty]:before{content:"☐台東縣"}[language=English] [select=true][i18n=taitungCounty]:before{content:"☑Taitung County"}[language=English] [select=false][i18n=taitungCounty]:before{content:"☐Taitung County"}</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormTaitungCounty</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="F28" s="7" t="str">
         <f t="shared" si="2"/>
@@ -10593,7 +11162,7 @@
         <v>Taitung County</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>208</v>
+        <v>233</v>
       </c>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
@@ -10621,14 +11190,14 @@
         <v>[language=Chinese] [select=true][i18n=hualienCounty]:before{content:"☑花蓮縣"}[language=Chinese] [select=false][i18n=hualienCounty]:before{content:"☐花蓮縣"}[language=English] [select=true][i18n=hualienCounty]:before{content:"☑Hualien County"}[language=English] [select=false][i18n=hualienCounty]:before{content:"☐Hualien County"}</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>209</v>
+        <v>234</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="3"/>
         <v>dataFormHualienCounty</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
       <c r="F29" s="7" t="str">
         <f t="shared" si="2"/>
@@ -10639,7 +11208,7 @@
         <v>Hualien County</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>

</xml_diff>

<commit_message>
1106 - add login form, fix rebuild table bug, finsh datamember table query
</commit_message>
<xml_diff>
--- a/others/Web-Page-Design-i18n.xlsx
+++ b/others/Web-Page-Design-i18n.xlsx
@@ -2091,13 +2091,14 @@
     <row r="3">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:A26" si="1"> if(C3 = "index", "&lt;?php $tableQuery = &lt;&lt;&lt;EOD", 
+  if(or(C3 = "A00", C3 = "P00"), ""&amp;REPT(char(32), 4)&amp;"DROP TABLE IF EXISTS `"&amp;LOWER($B4)&amp;"`;",
   if(or(C3 = "A01", C3 = "P01"), ""&amp;REPT(char(32), 4)&amp;"CREATE TABLE IF NOT EXISTS `"&amp;LOWER($B3)&amp;"` (",
   if(or(C3 = "N00", C3 = "Z00"), ""&amp;REPT(char(32), 4)&amp;") ENGINE=InnoDB DEFAULT CHARSET=utf8 COLLATE=utf8_general_ci;",
   if(E3 = "primaryKey", ""&amp;REPT(char(32), 8)&amp;"`"&amp;B3&amp;"` int(64) NOT NULL,",
   if(or(E3 = "dateOfApplication", E3 = "accountCreationDate"),  ""&amp;REPT(char(32), 8)&amp;"`"&amp;B3&amp;"` timestamp NOT NULL DEFAULT current_timestamp() ON UPDATE current_timestamp() COMMENT '"&amp;H3&amp;"',",
   if(and(or(G3 = "choice", G3 = "text"), or(C4 = "N00", C4 = "Z00")), ""&amp;REPT(char(32), 8)&amp;"`"&amp;B3&amp;"` tinytext NOT NULL COMMENT '"&amp;H3&amp;"'",
   if(or(G3 = "choice", G3 = "text"), ""&amp;REPT(char(32), 8)&amp;"`"&amp;B3&amp;"` tinytext NOT NULL COMMENT '"&amp;H3&amp;"',",
-  if(and(or(C2 = "N00", C2 = "Z00"), C4 = ""), "EOD ?&gt;", ""))))))))</f>
+  if(and(or(C2 = "N00", C2 = "Z00"), C4 = ""), "EOD ?&gt;", "")))))))))</f>
         <v>&lt;?php $tableQuery = &lt;&lt;&lt;EOD</v>
       </c>
       <c r="B3" s="4" t="str">
@@ -2132,7 +2133,7 @@
     <row r="4">
       <c r="A4" s="1" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>    DROP TABLE IF EXISTS `dataform`;</v>
       </c>
       <c r="B4" s="4" t="str">
         <f>columns!A4</f>
@@ -2574,7 +2575,7 @@
     <row r="17">
       <c r="A17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>    DROP TABLE IF EXISTS `datamember`;</v>
       </c>
       <c r="B17" s="4" t="str">
         <f>columns!A17</f>

</xml_diff>